<commit_message>
Pending - Solved RLS Problem
Test In lab to verify
</commit_message>
<xml_diff>
--- a/minimumVarianceControl/RLS.xlsx
+++ b/minimumVarianceControl/RLS.xlsx
@@ -15,6 +15,35 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$J$5:$J$6</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$F$34</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>ut</t>
   </si>
@@ -405,11 +434,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="295825456"/>
-        <c:axId val="295824336"/>
+        <c:axId val="298474560"/>
+        <c:axId val="298472320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="295825456"/>
+        <c:axId val="298474560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,12 +495,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295824336"/>
+        <c:crossAx val="298472320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="295824336"/>
+        <c:axId val="298472320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295825456"/>
+        <c:crossAx val="298474560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -592,6 +621,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1929,11 +1959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292410304"/>
-        <c:axId val="292411984"/>
+        <c:axId val="299761520"/>
+        <c:axId val="299763760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292410304"/>
+        <c:axId val="299761520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,12 +2020,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292411984"/>
+        <c:crossAx val="299763760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292411984"/>
+        <c:axId val="299763760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2052,7 +2082,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292410304"/>
+        <c:crossAx val="299761520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2066,6 +2096,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3248,13 +3279,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3577,18 +3608,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3602,7 +3633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3615,14 +3646,23 @@
       <c r="D2" s="1">
         <v>65</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2">
+        <f>($J$5*C2)+($J$6*B2)</f>
+        <v>65.000981662906156</v>
+      </c>
+      <c r="F2" s="1">
+        <f>(E2-D2)^2</f>
+        <v>9.6366206132281813E-7</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3635,14 +3675,23 @@
       <c r="D3" s="1">
         <v>78.5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3">
+        <f t="shared" ref="E3:E32" si="0">($J$5*C3)+($J$6*B3)</f>
+        <v>78.500818876501953</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F32" si="1">(E3-D3)^2</f>
+        <v>6.7055872545005939E-7</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3655,8 +3704,17 @@
       <c r="D4" s="1">
         <v>90.65</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>90.650672368738171</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5207972006175421E-7</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3669,8 +3727,23 @@
       <c r="D5" s="1">
         <v>101.58500000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>101.58554051175078</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9215295272113558E-7</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>0.89998914757305348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3683,8 +3756,23 @@
       <c r="D6" s="1">
         <v>111.4265</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>111.42692184046213</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7794937548509401E-7</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>0.50003810710633689</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3697,8 +3785,17 @@
       <c r="D7" s="1">
         <v>120.28385</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>120.28416503630233</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>9.9247871782741861E-8</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3711,8 +3808,17 @@
       <c r="D8" s="1">
         <v>128.25546500000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>128.25568391255851</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7922708266748646E-8</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3725,8 +3831,17 @@
       <c r="D9" s="1">
         <v>135.42991850000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>135.43005090118908</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7530074865323472E-8</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3739,8 +3854,17 @@
       <c r="D10" s="1">
         <v>141.88692665000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>141.88698119095659</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>2.974715943447525E-9</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3753,8 +3877,17 @@
       <c r="D11" s="1">
         <v>147.698233985</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>147.69821845174738</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4128193701686264E-10</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3767,8 +3900,17 @@
       <c r="D12" s="1">
         <v>152.92841058650001</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>152.928331986459</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.1779664463568518E-9</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3781,8 +3923,17 @@
       <c r="D13" s="1">
         <v>157.63556952785001</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>157.63543416769954</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8322370334208704E-8</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3795,8 +3946,17 @@
       <c r="D14" s="1">
         <v>161.87201257506501</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>161.87182613081603</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4761457978403456E-8</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3809,8 +3969,17 @@
       <c r="D15" s="1">
         <v>165.68481131755851</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>165.68457889762084</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>5.4019027428582122E-8</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3823,8 +3992,17 @@
       <c r="D16" s="1">
         <v>169.11633018580267</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>169.11605638774518</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4965376286424533E-8</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3837,8 +4015,17 @@
       <c r="D17" s="1">
         <v>172.20469716722241</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>172.2043861288571</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6744864695263417E-8</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3851,8 +4038,17 @@
       <c r="D18" s="1">
         <v>174.98422745050016</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>174.98388289585779</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1871790157714157E-7</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3865,8 +4061,17 @@
       <c r="D19" s="1">
         <v>177.48580470545014</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>177.48542998615841</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4041454759267518E-7</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3879,8 +4084,17 @@
       <c r="D20" s="1">
         <v>179.73722423490511</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>179.736822367429</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6149746835835556E-7</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3893,8 +4107,17 @@
       <c r="D21" s="1">
         <v>181.76350181141461</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>181.76307551057249</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8173240799385673E-7</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3907,8 +4130,17 @@
       <c r="D22" s="1">
         <v>183.58715163027315</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>183.58670333940165</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0096470547321676E-7</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3921,8 +4153,17 @@
       <c r="D23" s="1">
         <v>185.22843646724584</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>185.22796838534794</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1910066314804462E-7</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3935,8 +4176,17 @@
       <c r="D24" s="1">
         <v>186.70559282052128</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>186.70510692669956</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3609280598398013E-7</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3949,8 +4199,17 @@
       <c r="D25" s="1">
         <v>188.03503353846915</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>188.03453161391604</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>2.5192825701059446E-7</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3963,8 +4222,17 @@
       <c r="D26" s="1">
         <v>189.23153018462224</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>189.23101383241084</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>2.666196062238681E-7</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3977,8 +4245,17 @@
       <c r="D27" s="1">
         <v>190.30837716616003</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>190.30784782905619</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8019776950378723E-7</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3991,8 +4268,17 @@
       <c r="D28" s="1">
         <v>191.27753944954404</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>191.27699842603698</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9270643518523225E-7</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4005,8 +4291,17 @@
       <c r="D29" s="1">
         <v>192.14978550458963</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>192.14923396331972</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0419777241831336E-7</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4019,8 +4314,17 @@
       <c r="D30" s="1">
         <v>192.93480695413066</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>192.93424594687417</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1472914183829619E-7</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4033,8 +4337,17 @@
       <c r="D31" s="1">
         <v>193.64132625871761</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>193.64075673207316</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2436059874389199E-7</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4046,6 +4359,21 @@
       </c>
       <c r="D32" s="1">
         <v>194.27719363284587</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>194.27661643875228</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3315302166380716E-7</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="1">
+        <f>SUM(F2:F32)</f>
+        <v>6.6357236537204379E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>